<commit_message>
Fix bugs in Excel src/dst
</commit_message>
<xml_diff>
--- a/engine/testing/template.xlsx
+++ b/engine/testing/template.xlsx
@@ -38,6 +38,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -59,18 +60,21 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFF8080"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -218,7 +222,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="I32" activeCellId="0" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65"/>
@@ -237,10 +241,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="3"/>
     </row>
-    <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>